<commit_message>
Added BESS degradation to NPV
</commit_message>
<xml_diff>
--- a/Data/ReferenceCase/CAPEX.xlsx
+++ b/Data/ReferenceCase/CAPEX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/Reference Case/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/ReferenceCase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{986306A8-99BB-4C6C-BD11-7F1EF21AFB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A1074A2-0D3F-4A95-AC21-FCF26F5ADC15}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{986306A8-99BB-4C6C-BD11-7F1EF21AFB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C9867D6-04C2-414E-814F-37314AA4F13C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B000B0C4-52C2-4CB6-8ED2-BB996655927F}"/>
+    <workbookView minimized="1" xWindow="4380" yWindow="-11820" windowWidth="14400" windowHeight="7275" xr2:uid="{B000B0C4-52C2-4CB6-8ED2-BB996655927F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Technology</t>
   </si>
@@ -90,14 +90,18 @@
   </si>
   <si>
     <t>Annualized Investment Cost [EUR/GW]</t>
+  </si>
+  <si>
+    <t>Annualized Investment Cost [EUR/kW]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -137,10 +141,12 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1450AC7-1667-414A-8432-AB1F5663E49B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,7 +499,7 @@
     <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,18 +518,21 @@
       <c r="F1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2839</v>
+        <v>2800</v>
       </c>
       <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>0.06</v>
       </c>
       <c r="E2" s="1">
@@ -532,20 +541,24 @@
       </c>
       <c r="F2" s="2">
         <f>B2*E2*1000000</f>
-        <v>222085653.00464574</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>219034810.99436706</v>
+      </c>
+      <c r="G2" s="4">
+        <f>B2*E2</f>
+        <v>219.03481099436706</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1632</v>
+        <v>1600</v>
       </c>
       <c r="C3">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>3.9E-2</v>
       </c>
       <c r="E3" s="1">
@@ -554,20 +567,24 @@
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F13" si="1">B3*E3*1000000</f>
-        <v>103366245.08144756</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>101339455.96220349</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G13" si="2">B3*E3</f>
+        <v>101.33945596220349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4815.72</v>
+        <v>4631</v>
       </c>
       <c r="C4">
         <v>25</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E4" s="1">
@@ -576,20 +593,24 @@
       </c>
       <c r="F4" s="2">
         <f t="shared" si="1"/>
-        <v>314814425.84496474</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>302738864.81938976</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="2"/>
+        <v>302.73886481938973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2242</v>
+        <v>2200</v>
       </c>
       <c r="C5">
         <v>40</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="E5" s="1">
@@ -598,20 +619,24 @@
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>164279124.7686927</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>161201638.9344888</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="2"/>
+        <v>161.20163893448881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2037</v>
+        <v>2000</v>
       </c>
       <c r="C6">
         <v>30</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="E6" s="1">
@@ -620,20 +645,24 @@
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>160868938.02797487</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>157946920.00783005</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="2"/>
+        <v>157.94692000783004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>595</v>
+        <v>837.5</v>
       </c>
       <c r="C7">
         <v>30</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="E7" s="1">
@@ -642,20 +671,24 @@
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>45092167.332476817</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>63470067.463780396</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="2"/>
+        <v>63.470067463780396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>900</v>
+        <v>1750</v>
       </c>
       <c r="C8">
         <v>30</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="E8" s="1">
@@ -664,20 +697,24 @@
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>71800556.617044076</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>139612193.42203018</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="2"/>
+        <v>139.61219342203017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>11100</v>
+        <v>11000</v>
       </c>
       <c r="C9">
         <v>45</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>7.8E-2</v>
       </c>
       <c r="E9" s="1">
@@ -686,20 +723,24 @@
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>896322496.92809165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>888247519.47828901</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="2"/>
+        <v>888.24751947828895</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="C10">
         <v>30</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="E10" s="1">
@@ -708,10 +749,14 @@
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>44203892.596835397</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>43497065.285938889</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="2"/>
+        <v>43.497065285938888</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -719,8 +764,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -728,13 +777,21 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>